<commit_message>
Fix mistake with moment of inertia for feet members -- don't need double-thickness feet after all.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -567,9 +567,6 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -587,9 +584,6 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -601,6 +595,18 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -950,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,14 +981,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <f>750</f>
         <v>750</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3">
@@ -991,13 +997,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E3">
@@ -1008,13 +1014,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B4">
         <v>500</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E4">
@@ -1025,7 +1031,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -1033,7 +1039,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B6">
@@ -1045,14 +1051,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B7">
         <f>structure!B4*structure!B3^3/12</f>
         <v>243000</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E7">
@@ -1060,14 +1066,14 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B8">
         <f>structure!B3/2</f>
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E8">
@@ -1079,33 +1085,32 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B9">
         <f>B6/2*B3/4</f>
         <v>20250</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <f>structure!E10*structure!B2/4</f>
-        <v>45380.231249999997</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="D9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E10">
+      <c r="E9">
         <f>structure!E7+structure!E8</f>
         <v>242.02789999999999</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <f>structure!E9*structure!B2/4</f>
+        <v>45380.231249999997</v>
+      </c>
+    </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B11">
@@ -1114,7 +1119,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="24" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="6">
@@ -1123,28 +1128,28 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="8">
-        <f>structure!E10/2</f>
+      <c r="B13" s="7">
+        <f>structure!E9/2</f>
         <v>121.01394999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <f>structure!B13*structure!B9/(structure!B7*structure!B4)</f>
         <v>2.0168991666666664E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <f>structure!E3/structure!B14</f>
         <v>94.204015322200462</v>
       </c>
@@ -1158,10 +1163,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E18">
@@ -1173,13 +1178,13 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B19">
         <v>25</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E19">
@@ -1190,7 +1195,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B20">
@@ -1199,7 +1204,7 @@
       <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="14" t="s">
         <v>34</v>
       </c>
       <c r="E20">
@@ -1211,7 +1216,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B21">
@@ -1219,7 +1224,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B22">
@@ -1231,14 +1236,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="11">
         <f>structure!B21*structure!B20^3/12</f>
         <v>79.309012499999994</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E23">
@@ -1246,14 +1251,14 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B24">
         <f>structure!B20/2</f>
         <v>1.335</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E24">
@@ -1265,14 +1270,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B25">
         <f>(structure!B20/2*structure!B21)*structure!B20/4</f>
         <v>44.555624999999999</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E25">
@@ -1281,14 +1286,14 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B26">
         <f>structure!E26*structure!B19</f>
         <v>3025.3487499999997</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="14" t="s">
         <v>39</v>
       </c>
       <c r="E26">
@@ -1297,14 +1302,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B27">
         <f>structure!B26*structure!B24/structure!B23</f>
         <v>50.925367167445188</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="20" t="s">
         <v>40</v>
       </c>
       <c r="E27">
@@ -1312,7 +1317,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="24" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="6">
@@ -1321,7 +1326,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B29">
@@ -1330,7 +1335,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B30">
@@ -1339,21 +1344,21 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <f>structure!E20/structure!B30</f>
         <v>106.64059804675409</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B34">
@@ -1361,7 +1366,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B35">
@@ -1369,7 +1374,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B36">
@@ -1377,7 +1382,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B37">
@@ -1386,16 +1391,16 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="11">
         <f>structure!B36*structure!B35^3/12</f>
         <v>79.309012499999994</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B39">
@@ -1404,7 +1409,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B40">
@@ -1413,7 +1418,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B41">
@@ -1422,7 +1427,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B42">
@@ -1431,21 +1436,21 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="9">
         <f>E20/B42</f>
         <v>6.0671152204961984E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B46">
@@ -1453,7 +1458,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B47">
@@ -1461,7 +1466,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B48">
@@ -1469,7 +1474,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B49">
@@ -1478,7 +1483,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B50">
@@ -1487,7 +1492,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="14" t="s">
         <v>49</v>
       </c>
       <c r="B51">
@@ -1496,7 +1501,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="6">
@@ -1504,403 +1509,403 @@
         <v>275.79465012091583</v>
       </c>
     </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55">
+        <v>11.8</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>18</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56">
+        <v>130</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57">
+        <v>125</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E57">
+        <f>structure!E9</f>
+        <v>242.02789999999999</v>
+      </c>
+      <c r="F57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58">
+        <v>600</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58">
+        <f>structure!B2/2</f>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59">
+        <f>structure!B56*structure!B57</f>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60">
+        <f>structure!B57*structure!B56^3/12</f>
+        <v>60750</v>
+      </c>
+    </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>52</v>
+      <c r="A62" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E63">
-        <v>11.8</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>9</v>
+      <c r="A63" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63">
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="B64">
         <v>18</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E64">
-        <v>130</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <f>2*structure!B64*structure!B63</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <f>2*structure!B64*structure!B63^3/12</f>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B65">
-        <v>125</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E65">
-        <f>structure!E10</f>
-        <v>242.02789999999999</v>
-      </c>
-      <c r="F65" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
+      <c r="B71">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B66">
+      <c r="B72">
         <v>600</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E66">
-        <f>structure!B2/2</f>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B67">
-        <f>structure!B64*structure!B65</f>
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73">
+        <f>2*structure!B70*structure!B71</f>
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74">
+        <f>2*structure!B71*structure!B70^3/12</f>
+        <v>29646</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" s="12">
+        <f>(structure!B59*(structure!B56/2)+structure!B66*(structure!B63/2+structure!B56)+structure!B73*(structure!B70/2+structure!B63+structure!B56))/(structure!B59+structure!B66+structure!B73)</f>
+        <v>35.391608391608393</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B68">
-        <f>structure!B65*structure!B64^3/12</f>
-        <v>60750</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B71">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B72">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B73">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B74">
-        <f>2*structure!B72*structure!B71</f>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B75">
-        <f>2*structure!B72*structure!B71^3/12</f>
-        <v>375000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B78">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B78" s="13">
+        <f>(structure!B60+structure!B67+structure!B74)+(structure!B59*(structure!B77-structure!B56/2)^2)+(structure!B66*(structure!B63/2+structure!B56-structure!B77)^2)+(structure!B73*(structure!B56+structure!B63+structure!B70/2-structure!B77)^2)</f>
+        <v>4037678.5174825173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B79">
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="B79" s="12">
+        <f>MAX(structure!B77,structure!B56+structure!B63+structure!B70-structure!B77)</f>
+        <v>50.608391608391607</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B80">
-        <v>600</v>
+        <f>structure!E57*structure!E58/2</f>
+        <v>45380.231249999997</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B81">
-        <f>2*structure!B78*structure!B79</f>
-        <v>1098</v>
+        <f>structure!B80*structure!B79/structure!B78</f>
+        <v>0.56879726913258755</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B82">
-        <f>2*structure!B79*structure!B78^3/12</f>
-        <v>29646</v>
+      <c r="A82" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82" s="6">
+        <f>structure!E56/structure!B81</f>
+        <v>228.55243345005721</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="11" t="s">
-        <v>66</v>
+      <c r="A84" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B85" s="13">
-        <f>(structure!B67*(structure!B64/2)+structure!B74*(structure!B71/2+structure!B64)+structure!B81*(structure!B78/2+structure!B71+structure!B64))/(structure!B67+structure!B74+structure!B81)</f>
-        <v>35.391608391608393</v>
+        <v>70</v>
+      </c>
+      <c r="B85">
+        <v>250</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E85">
+        <v>11.8</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B86" s="14">
-        <f>(structure!B68+structure!B75+structure!B82)+(structure!B67*(structure!B85-structure!B64/2)^2)+(structure!B74*(structure!B71/2+structure!B64-structure!B85)^2)+(structure!B81*(structure!B64+structure!B71+structure!B78/2-structure!B85)^2)</f>
-        <v>4037678.5174825173</v>
+        <v>59</v>
+      </c>
+      <c r="B86">
+        <v>50</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E86">
+        <v>130</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B87" s="13">
-        <f>MAX(structure!B85,structure!B64+structure!B71+structure!B78-structure!B85)</f>
-        <v>50.608391608391607</v>
+        <v>71</v>
+      </c>
+      <c r="B87">
+        <v>18</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E87">
+        <f>structure!E25</f>
+        <v>242.02789999999999</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="B88">
-        <f>structure!E65*structure!E66/2</f>
-        <v>45380.231249999997</v>
+        <f>structure!B87*structure!B86*2</f>
+        <v>1800</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E88">
+        <f>structure!B85</f>
+        <v>250</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B89">
+        <f>structure!B87*structure!B86^3/12*2</f>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90">
+        <f>structure!B86/2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91">
+        <f>(B88/2)*B86/4</f>
+        <v>11250</v>
+      </c>
+      <c r="C91" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92">
+        <f>structure!E87*structure!E88</f>
+        <v>60506.974999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B89">
-        <f>structure!B88*structure!B87/structure!B86</f>
-        <v>0.56879726913258755</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B90" s="6">
-        <f>structure!E64/structure!B89</f>
-        <v>228.55243345005721</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="15" t="s">
-        <v>70</v>
-      </c>
       <c r="B93">
-        <v>250</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E93">
-        <v>11.8</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>9</v>
+        <f>structure!B92*structure!B90/structure!B89</f>
+        <v>4.0337983333333334</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B94">
-        <v>50</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E94">
-        <v>130</v>
-      </c>
-      <c r="F94" s="4" t="s">
-        <v>9</v>
+      <c r="A94" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B94" s="9">
+        <f>structure!E86/structure!B93</f>
+        <v>32.227689452331738</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="15" t="s">
-        <v>71</v>
+      <c r="A95" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B95">
-        <v>18</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E95">
-        <f>structure!E25</f>
+        <f>E87</f>
         <v>242.02789999999999</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="15" t="s">
-        <v>63</v>
+      <c r="A96" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B96">
-        <f>structure!B95*structure!B94*2</f>
-        <v>1800</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E96">
-        <f>structure!B93</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B97">
-        <f>structure!B95*structure!B94^3/12*2</f>
-        <v>375000</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B98">
-        <f>structure!B94/2</f>
+        <f>B95*B91/(B89*B87)</f>
+        <v>0.40337983333333333</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B99">
-        <f>(B96/2)*B94/4</f>
-        <v>11250</v>
-      </c>
-      <c r="C99" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B100">
-        <f>structure!E95*structure!E96</f>
-        <v>60506.974999999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B101">
-        <f>structure!B100*structure!B98/structure!B97</f>
-        <v>4.0337983333333334</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="B102" s="10">
-        <f>structure!E94/structure!B101</f>
-        <v>32.227689452331738</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B103">
-        <f>E95</f>
-        <v>242.02789999999999</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B104">
-        <f>B103*B99/(B97*B95)</f>
-        <v>0.40337983333333333</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B105" s="24">
-        <f>E93/B104</f>
+      <c r="B97" s="22">
+        <f>E85/B96</f>
         <v>29.252825810578038</v>
       </c>
     </row>
@@ -1908,10 +1913,10 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
     <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F63" r:id="rId3"/>
-    <hyperlink ref="F64" r:id="rId4"/>
-    <hyperlink ref="F93" r:id="rId5"/>
-    <hyperlink ref="F94" r:id="rId6"/>
+    <hyperlink ref="F55" r:id="rId3"/>
+    <hyperlink ref="F56" r:id="rId4"/>
+    <hyperlink ref="F85" r:id="rId5"/>
+    <hyperlink ref="F86" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1922,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1946,7 +1951,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B16" t="s">
@@ -1957,13 +1962,13 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E17">
@@ -1975,13 +1980,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B18">
         <v>2.67</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E18">
@@ -1992,13 +1997,13 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="14" t="s">
         <v>82</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="14" t="s">
         <v>34</v>
       </c>
       <c r="E19">
@@ -2010,7 +2015,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="14" t="s">
         <v>83</v>
       </c>
       <c r="B20">
@@ -2019,7 +2024,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="14" t="s">
         <v>84</v>
       </c>
       <c r="B21">
@@ -2031,14 +2036,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <f>E25/B21</f>
         <v>2.2661788389513107</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E22">
@@ -2046,14 +2051,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="16">
         <f>E18/B22</f>
         <v>110.31786004836633</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E23">
@@ -2065,7 +2070,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E24">
@@ -2074,7 +2079,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="14" t="s">
         <v>39</v>
       </c>
       <c r="E25">
@@ -2088,7 +2093,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B28" t="s">
@@ -2099,13 +2104,13 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="14" t="s">
         <v>89</v>
       </c>
       <c r="B29">
         <v>125</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E29">
@@ -2116,13 +2121,13 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="14" t="s">
         <v>90</v>
       </c>
       <c r="B30">
         <v>18</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E30">
@@ -2133,13 +2138,13 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B31">
         <v>12.5</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="14" t="s">
         <v>92</v>
       </c>
       <c r="E31">
@@ -2147,19 +2152,19 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="11">
         <f>B29/3</f>
         <v>41.666666666666664</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="11">
         <f>B32*B31</f>
         <v>520.83333333333326</v>
       </c>
@@ -2168,14 +2173,14 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B34">
         <f>B29/3</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="14" t="s">
         <v>97</v>
       </c>
       <c r="E34">
@@ -2184,14 +2189,14 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B35">
         <f>B32*3</f>
         <v>125</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="14" t="s">
         <v>99</v>
       </c>
       <c r="E35">
@@ -2200,14 +2205,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B36">
         <f>B35*B30^3/12</f>
         <v>60750</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="14" t="s">
         <v>39</v>
       </c>
       <c r="E36">
@@ -2216,14 +2221,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B37">
         <f>B30/2</f>
         <v>9</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="14" t="s">
         <v>101</v>
       </c>
       <c r="E37">
@@ -2232,14 +2237,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B38">
         <f>E38*B31</f>
         <v>1815.2092499999999</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="14" t="s">
         <v>102</v>
       </c>
       <c r="E38">
@@ -2248,7 +2253,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B39">
@@ -2257,16 +2262,16 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="9">
         <f>E30/B39</f>
         <v>483.41534178497608</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="14" t="s">
         <v>85</v>
       </c>
       <c r="B41">
@@ -2275,16 +2280,16 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="9">
         <f>E31/B41</f>
         <v>38.735203668667957</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B44" t="s">
@@ -2295,13 +2300,13 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="14" t="s">
         <v>89</v>
       </c>
       <c r="B45">
         <v>125</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="14" t="s">
         <v>107</v>
       </c>
       <c r="E45">
@@ -2309,13 +2314,13 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B46">
         <v>50</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E46">
@@ -2327,13 +2332,13 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B47">
         <v>18</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="14" t="s">
         <v>101</v>
       </c>
       <c r="E47">
@@ -2342,14 +2347,14 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="12">
+      <c r="B48" s="11">
         <f>B45/3</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="14" t="s">
         <v>102</v>
       </c>
       <c r="E48">
@@ -2358,16 +2363,16 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B49" s="11">
         <f>B48*B46</f>
         <v>2083.333333333333</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B50">
@@ -2376,7 +2381,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B51">
@@ -2385,7 +2390,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="14" t="s">
         <v>110</v>
       </c>
       <c r="B52">
@@ -2394,7 +2399,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B53">
@@ -2403,7 +2408,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B54">
@@ -2412,7 +2417,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B55">
@@ -2421,16 +2426,16 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B56" s="10">
+      <c r="B56" s="9">
         <f>E30/B55</f>
         <v>12.085383544624401</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="14" t="s">
         <v>85</v>
       </c>
       <c r="B57">
@@ -2439,10 +2444,10 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="10">
+      <c r="B58" s="9">
         <f>E31/B57</f>
         <v>15.494081467467179</v>
       </c>
@@ -2453,22 +2458,22 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="18" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="21" t="s">
+      <c r="A62" s="19" t="s">
         <v>112</v>
       </c>
       <c r="B62">
         <f>111-10</f>
         <v>101</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="20" t="s">
         <v>119</v>
       </c>
       <c r="E62">
@@ -2476,13 +2481,13 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B63">
         <v>5</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="20" t="s">
         <v>118</v>
       </c>
       <c r="E63">
@@ -2494,7 +2499,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="20" t="s">
         <v>113</v>
       </c>
       <c r="B64">
@@ -2502,7 +2507,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="22" t="s">
+      <c r="A65" s="20" t="s">
         <v>82</v>
       </c>
       <c r="B65">
@@ -2513,14 +2518,14 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="20" t="s">
         <v>116</v>
       </c>
       <c r="B66">
         <f>PI()*B63^2/4</f>
         <v>19.634954084936208</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="14" t="s">
         <v>107</v>
       </c>
       <c r="E66">
@@ -2528,14 +2533,14 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="22" t="s">
+      <c r="A67" s="20" t="s">
         <v>115</v>
       </c>
       <c r="B67">
         <f>E69/B65</f>
         <v>299.53948019801982</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E67">
@@ -2544,14 +2549,14 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="22" t="s">
+      <c r="A68" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B68">
         <f>B67/B66</f>
         <v>15.255420455901362</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="14" t="s">
         <v>101</v>
       </c>
       <c r="E68">
@@ -2560,14 +2565,14 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="23" t="s">
+      <c r="A69" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B69" s="24">
+      <c r="B69" s="22">
         <f>E63/B68</f>
         <v>36.87869512520485</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="26" t="s">
         <v>114</v>
       </c>
       <c r="E69">
@@ -2576,7 +2581,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="17" t="s">
         <v>126</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2584,14 +2589,14 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="20" t="s">
         <v>113</v>
       </c>
       <c r="B72">
         <f>B64</f>
         <v>12</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E72">
@@ -2602,7 +2607,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="22" t="s">
+      <c r="A73" s="20" t="s">
         <v>121</v>
       </c>
       <c r="B73">
@@ -2611,7 +2616,7 @@
       <c r="C73" t="s">
         <v>124</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E73">
@@ -2622,14 +2627,14 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="22" t="s">
+      <c r="A74" s="20" t="s">
         <v>122</v>
       </c>
       <c r="B74">
         <f>B73*B63</f>
         <v>30</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="14" t="s">
         <v>92</v>
       </c>
       <c r="E74">
@@ -2637,7 +2642,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="22" t="s">
+      <c r="A75" s="20" t="s">
         <v>123</v>
       </c>
       <c r="B75">
@@ -2646,24 +2651,24 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="23" t="s">
+      <c r="A76" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="24">
+      <c r="B76" s="22">
         <f>E74/B75</f>
         <v>1.0816604201416449</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="18" t="s">
+      <c r="A78" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D78" s="20" t="s">
+      <c r="D78" s="18" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="22" t="s">
+      <c r="A79" s="20" t="s">
         <v>127</v>
       </c>
       <c r="B79">
@@ -2672,7 +2677,7 @@
       <c r="C79" t="s">
         <v>134</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="20" t="s">
         <v>130</v>
       </c>
       <c r="E79">
@@ -2680,7 +2685,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="22" t="s">
+      <c r="A80" s="20" t="s">
         <v>128</v>
       </c>
       <c r="B80">
@@ -2689,7 +2694,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="22" t="s">
+      <c r="A81" s="20" t="s">
         <v>131</v>
       </c>
       <c r="B81">
@@ -2700,7 +2705,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="22" t="s">
+      <c r="A82" s="20" t="s">
         <v>133</v>
       </c>
       <c r="B82">
@@ -2709,16 +2714,16 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="B83" s="24">
+      <c r="B83" s="22">
         <f>B82/E69</f>
         <v>2.0030748521141568</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="18" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change bracket from Home Depot steel angle to glass fiber reinforced sandwich design
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="144">
   <si>
     <t>Desktop - simply supported</t>
   </si>
@@ -126,9 +126,6 @@
     <t>thickness (mm)</t>
   </si>
   <si>
-    <t>12-gauge plate</t>
-  </si>
-  <si>
     <t>shear yield strength (Mpa)</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>cantilever leg – torsion</t>
   </si>
   <si>
-    <t>approximate torsional constant, J_T (mm^3)</t>
-  </si>
-  <si>
     <t>max torque per bracket (Nmm)</t>
   </si>
   <si>
@@ -442,6 +436,27 @@
   </si>
   <si>
     <t>fixed leadscrew block to boxway</t>
+  </si>
+  <si>
+    <t>skin thickness (mm)</t>
+  </si>
+  <si>
+    <t>spacer thickness (mm)</t>
+  </si>
+  <si>
+    <t>I_width_bending (mm^4)</t>
+  </si>
+  <si>
+    <t>I_polar (mm^4)</t>
+  </si>
+  <si>
+    <t>Material: continuous glass fiber in nylon</t>
+  </si>
+  <si>
+    <t>average values provided by markforged</t>
+  </si>
+  <si>
+    <t>tensile strength (Mpa)</t>
   </si>
 </sst>
 </file>
@@ -956,23 +971,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.21875"/>
-    <col min="2" max="2" width="10.5546875"/>
-    <col min="3" max="3" width="16.44140625"/>
-    <col min="4" max="4" width="32.6640625"/>
-    <col min="5" max="5" width="12.77734375"/>
-    <col min="6" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="41.28515625"/>
+    <col min="2" max="2" width="10.5703125"/>
+    <col min="3" max="3" width="16.42578125"/>
+    <col min="4" max="4" width="32.7109375"/>
+    <col min="5" max="5" width="12.7109375"/>
+    <col min="6" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -980,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -996,7 +1011,7 @@
         <v>6.7999999999999995E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +1028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
@@ -1030,7 +1045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
@@ -1038,7 +1053,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
@@ -1050,7 +1065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
@@ -1065,7 +1080,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
@@ -1084,7 +1099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>18</v>
       </c>
@@ -1100,7 +1115,7 @@
         <v>242.02789999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -1109,7 +1124,7 @@
         <v>45380.231249999997</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>21</v>
       </c>
@@ -1118,7 +1133,7 @@
         <v>1.6807493055555556</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>22</v>
       </c>
@@ -1127,7 +1142,7 @@
         <v>17.849181850522193</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>23</v>
       </c>
@@ -1136,7 +1151,7 @@
         <v>121.01394999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
@@ -1145,7 +1160,7 @@
         <v>2.0168991666666664E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
@@ -1154,15 +1169,18 @@
         <v>94.204015322200462</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="E17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>28</v>
       </c>
@@ -1170,14 +1188,14 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <f>(7.8/1000)/10^3</f>
-        <v>7.7999999999999999E-6</v>
+        <f>(1.6/1000)/10^3</f>
+        <v>1.6000000000000001E-6</v>
       </c>
       <c r="F18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>30</v>
       </c>
@@ -1185,63 +1203,60 @@
         <v>25</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="E19">
-        <v>250</v>
+        <v>590</v>
       </c>
       <c r="F19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="B20">
-        <v>2.67</v>
-      </c>
-      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="E20">
         <f>0.58*structure!E19</f>
-        <v>145</v>
+        <v>342.2</v>
       </c>
       <c r="F20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="B21">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22">
+        <f>B3-2*B20</f>
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B22">
-        <f>structure!B20*structure!B21</f>
-        <v>133.5</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="11">
-        <f>structure!B21*structure!B20^3/12</f>
-        <v>79.309012499999994</v>
+      <c r="B23">
+        <f>2*B20*B21</f>
+        <v>270</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>14</v>
@@ -1250,13 +1265,13 @@
         <v>197</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24">
-        <f>structure!B20/2</f>
-        <v>1.335</v>
+        <v>13</v>
+      </c>
+      <c r="B24" s="11">
+        <f>(B21*(B22+2*B20)^3-B21*B22^3)/12</f>
+        <v>15390</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>16</v>
@@ -1266,16 +1281,16 @@
         <v>45.027900000000002</v>
       </c>
       <c r="F24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25">
-        <f>(structure!B20/2*structure!B21)*structure!B20/4</f>
-        <v>44.555624999999999</v>
+        <v>139</v>
+      </c>
+      <c r="B25" s="11">
+        <f>((B22+2*B20)*B21^3-B22*B21^3)/12</f>
+        <v>45562.5</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>20</v>
@@ -1285,627 +1300,636 @@
         <v>242.02789999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B26">
-        <f>structure!E26*structure!B19</f>
-        <v>3025.3487499999997</v>
+        <f>structure!B20/2</f>
+        <v>1.5</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26">
         <f>structure!E25/2</f>
         <v>121.01394999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B27">
-        <f>structure!B26*structure!B24/structure!B23</f>
-        <v>50.925367167445188</v>
+        <f>(structure!B20/2*structure!B21)*structure!B20/4</f>
+        <v>50.625</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27">
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <f>structure!E26*structure!B19</f>
+        <v>3025.3487499999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <f>structure!B28*structure!B26/structure!B24</f>
+        <v>0.29486829922027291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="6">
-        <f>structure!E19/structure!B27</f>
-        <v>4.9091447721523016</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+      <c r="B30" s="6">
+        <f>structure!E19/structure!B29</f>
+        <v>2000.8932854435377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B29">
+      <c r="B31">
         <f>structure!E26</f>
         <v>121.01394999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B30">
-        <f>structure!B29*structure!B25/(structure!B23*structure!B21)</f>
-        <v>1.3597073033707867</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
+      <c r="B32">
+        <f>structure!B31*structure!B27/(structure!B24*structure!B21)</f>
+        <v>8.8460489766081871E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="9">
-        <f>structure!E20/structure!B30</f>
-        <v>106.64059804675409</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+      <c r="B33" s="9">
+        <f>structure!E20/structure!B32</f>
+        <v>38683.936851908395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39">
+        <f>structure!B37*structure!B38</f>
+        <v>133.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="11">
+        <f>B24+B25</f>
+        <v>60952.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <f>SQRT((B37/2)^2+(B38/2)^2)</f>
+        <v>25.03561912555789</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35">
-        <v>2.67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37">
-        <f>structure!B35*structure!B36</f>
-        <v>133.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="11">
-        <f>structure!B36*structure!B35^3/12</f>
-        <v>79.309012499999994</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39">
-        <f>SQRT((B35/2)^2+(B36/2)^2)</f>
-        <v>25.03561912555789</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40">
-        <f>0.333*B36*B35^3</f>
-        <v>316.91881395000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41">
+      <c r="B42">
         <f>E26*E27/2</f>
         <v>30253.487499999999</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <f>B42*B41/B40</f>
+        <v>12.426312132723458</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="9">
+        <f>E20/B43</f>
+        <v>27.538339319422878</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B42">
-        <f>B41*B39/B40</f>
-        <v>2389.9331845578695</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="15" t="s">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="9">
-        <f>E20/B42</f>
-        <v>6.0671152204961984E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
+      <c r="B47">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50">
+        <f>structure!B48*structure!B49</f>
+        <v>133.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47">
-        <v>2.67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49">
-        <f>structure!B47*structure!B48</f>
-        <v>133.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50">
+      <c r="B51">
         <f>structure!E26</f>
         <v>121.01394999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="14" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52">
+        <f>structure!B51/structure!B50</f>
+        <v>0.90647153558052429</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="6">
+        <f>structure!E19/structure!B52</f>
+        <v>650.87537428536132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
-        <f>structure!B50/structure!B49</f>
-        <v>0.90647153558052429</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
+      <c r="D55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="6">
-        <f>structure!E19/structure!B51</f>
-        <v>275.79465012091583</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E55">
+      <c r="E56">
         <v>11.8</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>18</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E56">
-        <v>130</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>18</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57">
+        <v>130</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>125</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E57">
+      <c r="D58" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E58">
         <f>structure!E9</f>
         <v>242.02789999999999</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>600</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58">
-        <v>600</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E58">
+      <c r="E59">
         <f>structure!B2/2</f>
         <v>375</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B59">
-        <f>structure!B56*structure!B57</f>
+      <c r="B60">
+        <f>structure!B57*structure!B58</f>
         <v>2250</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <f>structure!B58*structure!B57^3/12</f>
+        <v>60750</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B60">
-        <f>structure!B57*structure!B56^3/12</f>
-        <v>60750</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="s">
+      <c r="B67">
+        <f>2*structure!B65*structure!B64</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63">
+      <c r="B68">
+        <f>2*structure!B65*structure!B64^3/12</f>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74">
+        <f>2*structure!B71*structure!B72</f>
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B75">
+        <f>2*structure!B72*structure!B71^3/12</f>
+        <v>29646</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B78" s="12">
+        <f>(structure!B60*(structure!B57/2)+structure!B67*(structure!B64/2+structure!B57)+structure!B74*(structure!B71/2+structure!B64+structure!B57))/(structure!B60+structure!B67+structure!B74)</f>
+        <v>35.391608391608393</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B79" s="13">
+        <f>(structure!B61+structure!B68+structure!B75)+(structure!B60*(structure!B78-structure!B57/2)^2)+(structure!B67*(structure!B64/2+structure!B57-structure!B78)^2)+(structure!B74*(structure!B57+structure!B64+structure!B71/2-structure!B78)^2)</f>
+        <v>4037678.5174825173</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80" s="12">
+        <f>MAX(structure!B78,structure!B57+structure!B64+structure!B71-structure!B78)</f>
+        <v>50.608391608391607</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81">
+        <f>structure!E58*structure!E59/2</f>
+        <v>45380.231249999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82">
+        <f>structure!B81*structure!B80/structure!B79</f>
+        <v>0.56879726913258755</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B83" s="6">
+        <f>structure!E57/structure!B82</f>
+        <v>228.55243345005721</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B65">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B66">
-        <f>2*structure!B64*structure!B63</f>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67">
-        <f>2*structure!B64*structure!B63^3/12</f>
-        <v>375000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B70">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B71">
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B73">
-        <f>2*structure!B70*structure!B71</f>
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B74">
-        <f>2*structure!B71*structure!B70^3/12</f>
-        <v>29646</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B77" s="12">
-        <f>(structure!B59*(structure!B56/2)+structure!B66*(structure!B63/2+structure!B56)+structure!B73*(structure!B70/2+structure!B63+structure!B56))/(structure!B59+structure!B66+structure!B73)</f>
-        <v>35.391608391608393</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B78" s="13">
-        <f>(structure!B60+structure!B67+structure!B74)+(structure!B59*(structure!B77-structure!B56/2)^2)+(structure!B66*(structure!B63/2+structure!B56-structure!B77)^2)+(structure!B73*(structure!B56+structure!B63+structure!B70/2-structure!B77)^2)</f>
-        <v>4037678.5174825173</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B79" s="12">
-        <f>MAX(structure!B77,structure!B56+structure!B63+structure!B70-structure!B77)</f>
-        <v>50.608391608391607</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B80">
-        <f>structure!E57*structure!E58/2</f>
-        <v>45380.231249999997</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B81">
-        <f>structure!B80*structure!B79/structure!B78</f>
-        <v>0.56879726913258755</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B82" s="6">
-        <f>structure!E56/structure!B81</f>
-        <v>228.55243345005721</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D84" s="1" t="s">
+      <c r="B86">
+        <v>250</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B85">
-        <v>250</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E85">
+      <c r="E86">
         <v>11.8</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B86">
-        <v>50</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E86">
-        <v>130</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B87">
+        <v>50</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E87">
+        <v>130</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B88">
         <v>18</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E87">
+      <c r="D88" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E88">
         <f>structure!E25</f>
         <v>242.02789999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B88">
-        <f>structure!B87*structure!B86*2</f>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B89">
+        <f>structure!B88*structure!B87*2</f>
         <v>1800</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D89" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E89">
+        <f>structure!B86</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B90">
+        <f>structure!B88*structure!B87^3/12*2</f>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B91">
+        <f>structure!B87/2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92">
+        <f>(B89/2)*B87/4</f>
+        <v>11250</v>
+      </c>
+      <c r="C92" t="s">
         <v>73</v>
       </c>
-      <c r="E88">
-        <f>structure!B85</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B89">
-        <f>structure!B87*structure!B86^3/12*2</f>
-        <v>375000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B90">
-        <f>structure!B86/2</f>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93">
+        <f>structure!E88*structure!E89</f>
+        <v>60506.974999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B94">
+        <f>structure!B93*structure!B91/structure!B90</f>
+        <v>4.0337983333333334</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B95" s="9">
+        <f>structure!E87/structure!B94</f>
+        <v>32.227689452331738</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96">
+        <f>E88</f>
+        <v>242.02789999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97">
+        <f>B96*B92/(B90*B88)</f>
+        <v>0.40337983333333333</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B91">
-        <f>(B88/2)*B86/4</f>
-        <v>11250</v>
-      </c>
-      <c r="C91" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B92">
-        <f>structure!E87*structure!E88</f>
-        <v>60506.974999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B93">
-        <f>structure!B92*structure!B90/structure!B89</f>
-        <v>4.0337983333333334</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B94" s="9">
-        <f>structure!E86/structure!B93</f>
-        <v>32.227689452331738</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B95">
-        <f>E87</f>
-        <v>242.02789999999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B96">
-        <f>B95*B91/(B89*B87)</f>
-        <v>0.40337983333333333</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B97" s="22">
-        <f>E85/B96</f>
+      <c r="B98" s="22">
+        <f>E86/B97</f>
         <v>29.252825810578038</v>
       </c>
     </row>
@@ -1913,10 +1937,10 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
     <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F55" r:id="rId3"/>
-    <hyperlink ref="F56" r:id="rId4"/>
-    <hyperlink ref="F85" r:id="rId5"/>
-    <hyperlink ref="F86" r:id="rId6"/>
+    <hyperlink ref="F56" r:id="rId3"/>
+    <hyperlink ref="F57" r:id="rId4"/>
+    <hyperlink ref="F86" r:id="rId5"/>
+    <hyperlink ref="F87" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1927,43 +1951,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45"/>
-    <col min="2" max="2" width="15.44140625"/>
-    <col min="3" max="3" width="8.5546875"/>
+    <col min="2" max="2" width="15.42578125"/>
+    <col min="3" max="3" width="8.5703125"/>
     <col min="4" max="4" width="42"/>
-    <col min="5" max="1025" width="8.5546875"/>
+    <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="B16" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>79</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -1979,9 +2003,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B18">
         <v>2.67</v>
@@ -1996,36 +2020,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19">
         <f>0.58*'joints and bearings'!E18</f>
         <v>145</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20">
         <f>B17*B18</f>
         <v>13.35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21">
         <f>B20*B19</f>
@@ -2035,9 +2059,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" s="12">
         <f>E25/B21</f>
@@ -2050,9 +2074,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="16">
         <f>E18/B22</f>
@@ -2069,7 +2093,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="14" t="s">
         <v>20</v>
       </c>
@@ -2078,40 +2102,40 @@
         <v>242.02789999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D25" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25">
         <f>'joints and bearings'!E24/2</f>
         <v>121.01394999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+      <c r="D28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>87</v>
-      </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>89</v>
       </c>
       <c r="B29">
         <v>125</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E29">
         <v>11.8</v>
@@ -2120,15 +2144,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30">
         <v>18</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E30">
         <v>130</v>
@@ -2137,90 +2161,90 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B31">
         <v>12.5</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E31">
         <v>10.8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B32" s="11">
         <f>B29/3</f>
         <v>41.666666666666664</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B33" s="11">
         <f>B32*B31</f>
         <v>520.83333333333326</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B34">
         <f>B29/3</f>
         <v>41.666666666666664</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E34">
         <f>50</f>
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B35">
         <f>B32*3</f>
         <v>125</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E35">
         <f>structure!B19</f>
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B36">
         <f>B35*B30^3/12</f>
         <v>60750</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E36">
         <f>E25</f>
         <v>121.01394999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>15</v>
       </c>
@@ -2229,14 +2253,14 @@
         <v>9</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E37">
         <f>E36*(E35+E34/2)</f>
         <v>6050.6974999999993</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>19</v>
       </c>
@@ -2245,14 +2269,14 @@
         <v>1815.2092499999999</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E38">
         <f>E37/B34</f>
         <v>145.21673999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>21</v>
       </c>
@@ -2261,61 +2285,61 @@
         <v>0.26891988888888885</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B40" s="9">
         <f>E30/B39</f>
         <v>483.41534178497608</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B41">
         <f>E38/B33</f>
         <v>0.2788161408</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B42" s="9">
         <f>E31/B41</f>
         <v>38.735203668667957</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45">
         <v>125</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E45">
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B46">
         <v>50</v>
@@ -2328,77 +2352,77 @@
         <v>242.02789999999999</v>
       </c>
       <c r="F46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B47">
         <v>18</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E47">
         <f>E46*E45</f>
         <v>60506.974999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B48" s="11">
         <f>B45/3</f>
         <v>41.666666666666664</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E48">
         <f>E47/B50</f>
         <v>1452.1674</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B49" s="11">
         <f>B48*B46</f>
         <v>2083.333333333333</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B50">
         <f>B45/3</f>
         <v>41.666666666666664</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B51">
         <f>B48*3</f>
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B52">
         <f>B51*B47^3/12</f>
         <v>60750</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>15</v>
       </c>
@@ -2407,7 +2431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>19</v>
       </c>
@@ -2416,7 +2440,7 @@
         <v>72608.37</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>21</v>
       </c>
@@ -2425,116 +2449,116 @@
         <v>10.756795555555556</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B56" s="9">
         <f>E30/B55</f>
         <v>12.085383544624401</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B57">
         <f>E48/B49</f>
         <v>0.69704035200000014</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B58" s="9">
         <f>E31/B57</f>
         <v>15.494081467467179</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B62">
         <f>111-10</f>
         <v>101</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E62">
         <v>970</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B63">
         <v>5</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E63">
         <f>0.58*E62</f>
         <v>562.59999999999991</v>
       </c>
       <c r="F63" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B64">
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B65">
         <v>2</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B66">
         <f>PI()*B63^2/4</f>
         <v>19.634954084936208</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E66">
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B67">
         <f>E69/B65</f>
@@ -2548,7 +2572,7 @@
         <v>242.02789999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>24</v>
       </c>
@@ -2557,47 +2581,47 @@
         <v>15.255420455901362</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E68">
         <f>E67*E66</f>
         <v>60506.974999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B69" s="22">
         <f>E63/B68</f>
         <v>36.87869512520485</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E69">
         <f>E68/B62</f>
         <v>599.07896039603963</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B72">
         <f>B64</f>
         <v>12</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E72">
         <v>11.8</v>
@@ -2606,18 +2630,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B73">
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E73">
         <v>130</v>
@@ -2626,105 +2650,105 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B74">
         <f>B73*B63</f>
         <v>30</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E74">
         <v>10.8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B75">
         <f>B67/B74</f>
         <v>9.9846493399339931</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B76" s="22">
         <f>E74/B75</f>
         <v>1.0816604201416449</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B79">
         <v>2000</v>
       </c>
       <c r="C79" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E79">
         <v>0.2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B80">
         <f>B79/(E79*B63)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B81">
         <v>0.3</v>
       </c>
       <c r="C81" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B82">
         <f>B80*B81*B65</f>
         <v>1200</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B83" s="22">
         <f>B82/E69</f>
         <v>2.0030748521141568</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix assembly errors for master assembly.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
@@ -973,7 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1951,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update detailed engineering to consider bolt preload pullthrough at column-to-feet joint and fixed bearing block-to-boxway joint.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="173">
   <si>
     <t>Desktop - simply supported</t>
   </si>
@@ -411,9 +411,6 @@
     <t>Bolt frictional characteristics</t>
   </si>
   <si>
-    <t>coefficient of friction - steel on brass</t>
-  </si>
-  <si>
     <t>coefficient of friction -- wood-to-wood</t>
   </si>
   <si>
@@ -457,6 +454,96 @@
   </si>
   <si>
     <t>tensile strength (Mpa)</t>
+  </si>
+  <si>
+    <t>coefficient of friction - steel on steel, lubricated</t>
+  </si>
+  <si>
+    <t>Loading on block: load per leadscrew, concentrated on one side</t>
+  </si>
+  <si>
+    <t>offset of edge from load (mm)</t>
+  </si>
+  <si>
+    <t>cross-sectional area per bolt (mm^2)</t>
+  </si>
+  <si>
+    <t>tensile load per bolt (N)</t>
+  </si>
+  <si>
+    <t>moment between fulcrum and bolts (Nmm)</t>
+  </si>
+  <si>
+    <t>max tensile stress in bolt (Mpa)</t>
+  </si>
+  <si>
+    <t>Safety Factor Until Bolt Breaks</t>
+  </si>
+  <si>
+    <t>bolts pullout -- worst case where preload completely relieved</t>
+  </si>
+  <si>
+    <t>max shear stress in bolt (Mpa)</t>
+  </si>
+  <si>
+    <t>Safety Factor Until Bolt Shears</t>
+  </si>
+  <si>
+    <t>bolt minor diameter (mm)</t>
+  </si>
+  <si>
+    <t>joint preload -- how far until above 2 cases become relevant</t>
+  </si>
+  <si>
+    <t>coefficient of friction -- aluminum-to-wood</t>
+  </si>
+  <si>
+    <t>sex bolt head diameter (mm)</t>
+  </si>
+  <si>
+    <t>sex bolt clearance hole diameter (mm)</t>
+  </si>
+  <si>
+    <t>sex bolt bearing area (mm^2)</t>
+  </si>
+  <si>
+    <t>5/16"</t>
+  </si>
+  <si>
+    <t>Safety Factor until wood locally crushed</t>
+  </si>
+  <si>
+    <t>bolt pull-through from preload</t>
+  </si>
+  <si>
+    <t>Safety Factor until bolt pulls through</t>
+  </si>
+  <si>
+    <t>boxway baseplate thickness (mm)</t>
+  </si>
+  <si>
+    <t>shear area (mm^2)</t>
+  </si>
+  <si>
+    <t>bolt hole radial crush -- worst case where clamping completely relieved</t>
+  </si>
+  <si>
+    <t>max shear stress in wood below bolt (Mpa)</t>
+  </si>
+  <si>
+    <t>shear stress in wood below bolt (Mpa)</t>
+  </si>
+  <si>
+    <t>flat head bolt head diameter (mm)</t>
+  </si>
+  <si>
+    <t>flat head bolt clearance hole diameter (mm)</t>
+  </si>
+  <si>
+    <t>flat head bolt bearing area (mm^2)</t>
+  </si>
+  <si>
+    <t>feet thickness (mm)</t>
   </si>
 </sst>
 </file>
@@ -467,7 +554,7 @@
     <numFmt numFmtId="164" formatCode="0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -548,6 +635,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -570,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -622,6 +714,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1174,10 +1275,10 @@
         <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" t="s">
         <v>141</v>
-      </c>
-      <c r="E17" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1203,7 +1304,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E19">
         <v>590</v>
@@ -1214,7 +1315,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1240,7 +1341,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22">
         <f>B3-2*B20</f>
@@ -1286,7 +1387,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25" s="11">
         <f>((B22+2*B20)*B21^3-B22*B21^3)/12</f>
@@ -1425,7 +1526,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B40" s="11">
         <f>B24+B25</f>
@@ -1899,7 +2000,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B95" s="9">
         <f>structure!E87/structure!B94</f>
@@ -1949,10 +2050,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,7 +2061,7 @@
     <col min="1" max="1" width="45"/>
     <col min="2" max="2" width="15.42578125"/>
     <col min="3" max="3" width="8.5703125"/>
-    <col min="4" max="4" width="42"/>
+    <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
@@ -2685,7 +2786,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D78" s="18" t="s">
         <v>127</v>
@@ -2699,13 +2800,13 @@
         <v>2000</v>
       </c>
       <c r="C79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="E79">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2714,41 +2815,505 @@
       </c>
       <c r="B80">
         <f>B79/(E79*B63)</f>
-        <v>2000</v>
+        <v>1333.3333333333333</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B81">
         <v>0.3</v>
       </c>
       <c r="C81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B82">
         <f>B80*B81*B65</f>
-        <v>1200</v>
+        <v>799.99999999999989</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B83" s="22">
         <f>B82/E69</f>
-        <v>2.0030748521141568</v>
+        <v>1.3353832347427712</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
-        <v>136</v>
+      <c r="A85" s="29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" s="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" s="30">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B88" s="30">
+        <f>PI()*(B86^2-B87^2)/4</f>
+        <v>78.885391531639698</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B89" s="30">
+        <f>B80/B88</f>
+        <v>16.902157768952115</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B90" s="31">
+        <f>E74/B89</f>
+        <v>0.63897167140628164</v>
+      </c>
+      <c r="C90" s="22"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B91" s="30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B92" s="30">
+        <f>B91*PI()*B86</f>
+        <v>678.58401317539528</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B93" s="30">
+        <f>B80/B92</f>
+        <v>1.9648758406406832</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B94" s="31">
+        <f>E72/B93</f>
+        <v>6.0054685166022486</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98">
+        <v>11.7</v>
+      </c>
+      <c r="D98" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E98">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B99">
+        <v>5</v>
+      </c>
+      <c r="D99" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E99">
+        <f>0.58*E98</f>
+        <v>562.59999999999991</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B102">
+        <f>PI()*B99^2/4</f>
+        <v>19.634954084936208</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E102">
+        <f>E46</f>
+        <v>242.02789999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B103">
+        <f>E104/B98/B101</f>
+        <v>217.20452564102567</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E103">
+        <f>12+9</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B104">
+        <f>B103/B102</f>
+        <v>11.06213565366386</v>
+      </c>
+      <c r="D104" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E104">
+        <f>E103*E102</f>
+        <v>5082.5859</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B105" s="22">
+        <f>E98/B104</f>
+        <v>87.686503797187555</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B106" s="28">
+        <f>E102/B101</f>
+        <v>121.01394999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B107" s="28">
+        <f>B106/B102</f>
+        <v>6.1631898641841492</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B108" s="22">
+        <f>E99/B107</f>
+        <v>91.283898824764492</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B109" s="28">
+        <f>B103/B133</f>
+        <v>0.25606795494592272</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B110" s="22">
+        <f>E113/B109</f>
+        <v>46.081517706860133</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>18</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B114">
+        <v>6</v>
+      </c>
+      <c r="C114" t="s">
+        <v>122</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E114">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B115">
+        <f>B114*B99</f>
+        <v>30</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E115">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B116">
+        <f>B106/B115</f>
+        <v>4.0337983333333334</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B117" s="22">
+        <f>E115/B116</f>
+        <v>2.6773772775783291</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D119" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B120">
+        <v>2000</v>
+      </c>
+      <c r="C120" t="s">
+        <v>131</v>
+      </c>
+      <c r="D120" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E120">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B121">
+        <f>B120/(E120*B99)</f>
+        <v>1333.3333333333333</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B122">
+        <v>0.3</v>
+      </c>
+      <c r="C122" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B123">
+        <f>B121*B122*B101</f>
+        <v>799.99999999999989</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124" s="22">
+        <f>B123/B103</f>
+        <v>3.6831645088379115</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B127" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B128" s="30">
+        <v>7.93</v>
+      </c>
+      <c r="C128" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B129" s="30">
+        <f>PI()*(B127^2-B128^2)/4</f>
+        <v>127.32490179899368</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B130" s="30">
+        <f>B121/B129</f>
+        <v>10.471897598148168</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B131" s="31">
+        <f>E115/B130</f>
+        <v>1.0313317045718489</v>
+      </c>
+      <c r="C131" s="22"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B132" s="30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B133" s="30">
+        <f>B132*PI()*B127</f>
+        <v>848.23001646924411</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B134" s="30">
+        <f>B121/B133</f>
+        <v>1.5719006725125466</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B135" s="31">
+        <f>E113/B134</f>
+        <v>7.5068356457528109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update detailed design spreadsheet for tip vs. slip analysis.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
     <sheet name="joints and bearings" sheetId="2" r:id="rId2"/>
+    <sheet name="tip vs. slip" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="180">
   <si>
     <t>Desktop - simply supported</t>
   </si>
@@ -544,6 +545,27 @@
   </si>
   <si>
     <t>feet thickness (mm)</t>
+  </si>
+  <si>
+    <t>Overdriving</t>
+  </si>
+  <si>
+    <t>Coefficient of friction, wood on wood</t>
+  </si>
+  <si>
+    <t>CG Height (mm)</t>
+  </si>
+  <si>
+    <t>approximating as midway up to first order</t>
+  </si>
+  <si>
+    <t>Mass of entire structure (kg)</t>
+  </si>
+  <si>
+    <t>Dead weight of structure (N)</t>
+  </si>
+  <si>
+    <t>Desktop height at top of travel (mm)</t>
   </si>
 </sst>
 </file>
@@ -2052,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,7 +2916,9 @@
         <f>E74/B89</f>
         <v>0.63897167140628164</v>
       </c>
-      <c r="C90" s="22"/>
+      <c r="C90" s="22" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="s">
@@ -3082,7 +3106,7 @@
       </c>
       <c r="B109" s="28">
         <f>B103/B133</f>
-        <v>0.25606795494592272</v>
+        <v>0.29546302493760312</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3091,7 +3115,7 @@
       </c>
       <c r="B110" s="22">
         <f>E113/B109</f>
-        <v>46.081517706860133</v>
+        <v>39.93731534594545</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3239,7 +3263,7 @@
         <v>157</v>
       </c>
       <c r="B127" s="30">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3259,7 +3283,7 @@
       </c>
       <c r="B129" s="30">
         <f>PI()*(B127^2-B128^2)/4</f>
-        <v>127.32490179899368</v>
+        <v>83.342604648736568</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3268,7 +3292,7 @@
       </c>
       <c r="B130" s="30">
         <f>B121/B129</f>
-        <v>10.471897598148168</v>
+        <v>15.998220105466141</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -3277,9 +3301,11 @@
       </c>
       <c r="B131" s="31">
         <f>E115/B130</f>
-        <v>1.0313317045718489</v>
-      </c>
-      <c r="C131" s="22"/>
+        <v>0.67507509765476637</v>
+      </c>
+      <c r="C131" s="22" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="20" t="s">
@@ -3295,7 +3321,7 @@
       </c>
       <c r="B133" s="30">
         <f>B132*PI()*B127</f>
-        <v>848.23001646924411</v>
+        <v>735.1326809400116</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -3304,7 +3330,7 @@
       </c>
       <c r="B134" s="30">
         <f>B121/B133</f>
-        <v>1.5719006725125466</v>
+        <v>1.8137315452067844</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -3313,7 +3339,7 @@
       </c>
       <c r="B135" s="31">
         <f>E113/B134</f>
-        <v>7.5068356457528109</v>
+        <v>6.5059242263191033</v>
       </c>
     </row>
   </sheetData>
@@ -3326,4 +3352,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2">
+        <v>300</v>
+      </c>
+      <c r="C2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3">
+        <v>8.7799999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4">
+        <f>B3*9.81</f>
+        <v>86.131799999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Complete tip vs. slip analysis.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="197">
   <si>
     <t>Desktop - simply supported</t>
   </si>
@@ -566,6 +566,57 @@
   </si>
   <si>
     <t>Desktop height at top of travel (mm)</t>
+  </si>
+  <si>
+    <t>Design live load (N)</t>
+  </si>
+  <si>
+    <t>from Solidworks</t>
+  </si>
+  <si>
+    <t>Feet support span (mm)</t>
+  </si>
+  <si>
+    <t>Desktop depth (mm)</t>
+  </si>
+  <si>
+    <t>Offset of CG from front edge (mm)</t>
+  </si>
+  <si>
+    <t>Offset of design load from front edge (mm)</t>
+  </si>
+  <si>
+    <t>From dead weight (Nmm)</t>
+  </si>
+  <si>
+    <t>From design load (Nmm)</t>
+  </si>
+  <si>
+    <t>Support force magnitude (N)</t>
+  </si>
+  <si>
+    <t>Max lateral load before sliding (N)</t>
+  </si>
+  <si>
+    <t>Support force offset from front edge at cusp of tipping (mm)</t>
+  </si>
+  <si>
+    <t>From support force (Nmm)</t>
+  </si>
+  <si>
+    <t>Moments about front edge of feet at cusp of tipping</t>
+  </si>
+  <si>
+    <t>Tolerable lateral load before tipping (N)</t>
+  </si>
+  <si>
+    <t>conservatively assume concentrated 3/4 of the way back</t>
+  </si>
+  <si>
+    <t>Factor of safety against tipping</t>
+  </si>
+  <si>
+    <t>3 Nm</t>
   </si>
 </sst>
 </file>
@@ -576,7 +627,7 @@
     <numFmt numFmtId="164" formatCode="0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -662,6 +713,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -684,7 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -745,6 +802,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1096,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2819,10 +2877,10 @@
         <v>125</v>
       </c>
       <c r="B79">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="C79" t="s">
-        <v>131</v>
+        <v>196</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>143</v>
@@ -2837,7 +2895,7 @@
       </c>
       <c r="B80">
         <f>B79/(E79*B63)</f>
-        <v>1333.3333333333333</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2857,7 +2915,7 @@
       </c>
       <c r="B82">
         <f>B80*B81*B65</f>
-        <v>799.99999999999989</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2866,7 +2924,7 @@
       </c>
       <c r="B83" s="22">
         <f>B82/E69</f>
-        <v>1.3353832347427712</v>
+        <v>2.0030748521141568</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2905,7 +2963,7 @@
       </c>
       <c r="B89" s="30">
         <f>B80/B88</f>
-        <v>16.902157768952115</v>
+        <v>25.353236653428173</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2914,7 +2972,7 @@
       </c>
       <c r="B90" s="31">
         <f>E74/B89</f>
-        <v>0.63897167140628164</v>
+        <v>0.42598111427085439</v>
       </c>
       <c r="C90" s="22" t="s">
         <v>173</v>
@@ -2943,7 +3001,7 @@
       </c>
       <c r="B93" s="30">
         <f>B80/B92</f>
-        <v>1.9648758406406832</v>
+        <v>2.9473137609610252</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2952,7 +3010,7 @@
       </c>
       <c r="B94" s="31">
         <f>E72/B93</f>
-        <v>6.0054685166022486</v>
+        <v>4.0036456777348324</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3356,15 +3414,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3372,7 +3431,7 @@
         <v>174</v>
       </c>
       <c r="B1">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3398,7 +3457,7 @@
       <c r="A4" t="s">
         <v>178</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="13">
         <f>B3*9.81</f>
         <v>86.131799999999998</v>
       </c>
@@ -3406,6 +3465,133 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>179</v>
+      </c>
+      <c r="B5" s="13">
+        <f>ROUNDUP(398.17,1)</f>
+        <v>398.20000000000005</v>
+      </c>
+      <c r="C5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6">
+        <f>structure!E7</f>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10">
+        <v>375</v>
+      </c>
+      <c r="C10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="13">
+        <f>B6+B4</f>
+        <v>283.1318</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" s="28">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="32">
+        <f>B1*(B6+B4)</f>
+        <v>70.78295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16">
+        <f>-B4*B9</f>
+        <v>-21532.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17">
+        <f>-B6*B10</f>
+        <v>-73875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18">
+        <f>B11*B12</f>
+        <v>141565.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="32">
+        <f>SUM(B16:B18)/B5</f>
+        <v>115.91649924660972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21" s="22">
+        <f>B19/B13</f>
+        <v>1.6376330634228966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update error budget and detailed structural calculations to account for mispositioned bolt holes.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shien\Dropbox (MIT)\Spring 2017\2.77\2-77-ppd\design_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (MIT)\Spring 2017\2.77\2-77-ppd\design_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
@@ -448,9 +448,6 @@
     <t>I_polar (mm^4)</t>
   </si>
   <si>
-    <t>Material: continuous glass fiber in nylon</t>
-  </si>
-  <si>
     <t>average values provided by markforged</t>
   </si>
   <si>
@@ -617,6 +614,9 @@
   </si>
   <si>
     <t>3 Nm</t>
+  </si>
+  <si>
+    <t>Material: steel</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,10 +1355,10 @@
         <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" t="s">
         <v>140</v>
-      </c>
-      <c r="E17" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1384,10 +1384,10 @@
         <v>25</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19">
-        <v>590</v>
+        <v>370</v>
       </c>
       <c r="F19" t="s">
         <v>29</v>
@@ -1398,14 +1398,14 @@
         <v>136</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E20">
         <f>0.58*structure!E19</f>
-        <v>342.2</v>
+        <v>214.6</v>
       </c>
       <c r="F20" t="s">
         <v>34</v>
@@ -1424,8 +1424,7 @@
         <v>137</v>
       </c>
       <c r="B22">
-        <f>B3-2*B20</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>36</v>
@@ -1437,7 +1436,7 @@
       </c>
       <c r="B23">
         <f>2*B20*B21</f>
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>14</v>
@@ -1452,7 +1451,7 @@
       </c>
       <c r="B24" s="11">
         <f>(B21*(B22+2*B20)^3-B21*B22^3)/12</f>
-        <v>15390</v>
+        <v>8130</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>16</v>
@@ -1471,7 +1470,7 @@
       </c>
       <c r="B25" s="11">
         <f>((B22+2*B20)*B21^3-B22*B21^3)/12</f>
-        <v>45562.5</v>
+        <v>15187.5</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>20</v>
@@ -1486,8 +1485,8 @@
         <v>15</v>
       </c>
       <c r="B26">
-        <f>structure!B20/2</f>
-        <v>1.5</v>
+        <f>(B22+2*B20)/2</f>
+        <v>10</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>38</v>
@@ -1503,7 +1502,7 @@
       </c>
       <c r="B27">
         <f>(structure!B20/2*structure!B21)*structure!B20/4</f>
-        <v>50.625</v>
+        <v>5.625</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>39</v>
@@ -1527,7 +1526,7 @@
       </c>
       <c r="B29">
         <f>structure!B28*structure!B26/structure!B24</f>
-        <v>0.29486829922027291</v>
+        <v>3.721216174661746</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1536,7 +1535,7 @@
       </c>
       <c r="B30" s="6">
         <f>structure!E19/structure!B29</f>
-        <v>2000.8932854435377</v>
+        <v>99.4298591195478</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1554,7 +1553,7 @@
       </c>
       <c r="B32">
         <f>structure!B31*structure!B27/(structure!B24*structure!B21)</f>
-        <v>8.8460489766081871E-3</v>
+        <v>1.8606080873308731E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1563,7 +1562,7 @@
       </c>
       <c r="B33" s="9">
         <f>structure!E20/structure!B32</f>
-        <v>38683.936851908395</v>
+        <v>115338.63657867545</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1583,7 @@
         <v>32</v>
       </c>
       <c r="B37">
-        <v>2.67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1592,7 +1591,7 @@
         <v>35</v>
       </c>
       <c r="B38">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1601,7 +1600,7 @@
       </c>
       <c r="B39">
         <f>structure!B37*structure!B38</f>
-        <v>133.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1610,7 +1609,7 @@
       </c>
       <c r="B40" s="11">
         <f>B24+B25</f>
-        <v>60952.5</v>
+        <v>23317.5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,7 +1618,7 @@
       </c>
       <c r="B41">
         <f>SQRT((B37/2)^2+(B38/2)^2)</f>
-        <v>25.03561912555789</v>
+        <v>22.5055548698538</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1637,7 +1636,7 @@
       </c>
       <c r="B43">
         <f>B42*B41/B40</f>
-        <v>12.426312132723458</v>
+        <v>29.200022426747552</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1645,7 @@
       </c>
       <c r="B44" s="9">
         <f>E20/B43</f>
-        <v>27.538339319422878</v>
+        <v>7.3493094239346872</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1667,7 +1666,7 @@
         <v>32</v>
       </c>
       <c r="B48">
-        <v>2.67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,7 +1683,7 @@
       </c>
       <c r="B50">
         <f>structure!B48*structure!B49</f>
-        <v>133.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1702,7 +1701,7 @@
       </c>
       <c r="B52">
         <f>structure!B51/structure!B50</f>
-        <v>0.90647153558052429</v>
+        <v>2.4202789999999998</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1711,7 +1710,7 @@
       </c>
       <c r="B53" s="6">
         <f>structure!E19/structure!B52</f>
-        <v>650.87537428536132</v>
+        <v>152.8749371456762</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2132,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2880,10 +2879,10 @@
         <v>3000</v>
       </c>
       <c r="C79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E79">
         <v>0.3</v>
@@ -2929,12 +2928,12 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B86" s="30">
         <v>12</v>
@@ -2942,7 +2941,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B87" s="30">
         <v>6.6</v>
@@ -2950,7 +2949,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B88" s="30">
         <f>PI()*(B86^2-B87^2)/4</f>
@@ -2968,19 +2967,19 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B90" s="31">
         <f>E74/B89</f>
         <v>0.42598111427085439</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B91" s="30">
         <v>18</v>
@@ -2988,7 +2987,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B92" s="30">
         <f>B91*PI()*B86</f>
@@ -2997,7 +2996,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B93" s="30">
         <f>B80/B92</f>
@@ -3006,7 +3005,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B94" s="31">
         <f>E72/B93</f>
@@ -3020,7 +3019,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D97" s="18" t="s">
         <v>115</v>
@@ -3042,7 +3041,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B99">
         <v>5</v>
@@ -3071,12 +3070,12 @@
         <v>2</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B102">
         <f>PI()*B99^2/4</f>
@@ -3092,14 +3091,14 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B103">
         <f>E104/B98/B101</f>
         <v>217.20452564102567</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E103">
         <f>12+9</f>
@@ -3108,14 +3107,14 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B104">
         <f>B103/B102</f>
         <v>11.06213565366386</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E104">
         <f>E103*E102</f>
@@ -3124,7 +3123,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B105" s="22">
         <f>E98/B104</f>
@@ -3142,7 +3141,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B107" s="28">
         <f>B106/B102</f>
@@ -3151,7 +3150,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B108" s="22">
         <f>E99/B107</f>
@@ -3160,7 +3159,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B109" s="28">
         <f>B103/B133</f>
@@ -3169,7 +3168,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B110" s="22">
         <f>E113/B109</f>
@@ -3178,7 +3177,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>50</v>
@@ -3250,7 +3249,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D119" s="18" t="s">
         <v>127</v>
@@ -3267,7 +3266,7 @@
         <v>131</v>
       </c>
       <c r="D120" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E120">
         <v>0.3</v>
@@ -3284,7 +3283,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B122">
         <v>0.3</v>
@@ -3313,12 +3312,12 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B127" s="30">
         <v>13</v>
@@ -3326,18 +3325,18 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B128" s="30">
         <v>7.93</v>
       </c>
       <c r="C128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B129" s="30">
         <f>PI()*(B127^2-B128^2)/4</f>
@@ -3355,19 +3354,19 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B131" s="31">
         <f>E115/B130</f>
         <v>0.67507509765476637</v>
       </c>
       <c r="C131" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B132" s="30">
         <v>18</v>
@@ -3375,7 +3374,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B133" s="30">
         <f>B132*PI()*B127</f>
@@ -3384,7 +3383,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B134" s="30">
         <f>B121/B133</f>
@@ -3393,7 +3392,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B135" s="31">
         <f>E113/B134</f>
@@ -3428,7 +3427,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1">
         <v>0.25</v>
@@ -3436,18 +3435,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2">
         <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3">
         <v>8.7799999999999994</v>
@@ -3455,7 +3454,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B4" s="13">
         <f>B3*9.81</f>
@@ -3464,19 +3463,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" s="13">
         <f>ROUNDUP(398.17,1)</f>
         <v>398.20000000000005</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B6">
         <f>structure!E7</f>
@@ -3485,7 +3484,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>500</v>
@@ -3493,7 +3492,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8">
         <v>500</v>
@@ -3501,7 +3500,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9">
         <v>250</v>
@@ -3509,18 +3508,18 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10">
         <v>375</v>
       </c>
       <c r="C10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11" s="13">
         <f>B6+B4</f>
@@ -3529,7 +3528,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="28">
         <v>500</v>
@@ -3537,7 +3536,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13" s="32">
         <f>B1*(B6+B4)</f>
@@ -3546,12 +3545,12 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B16">
         <f>-B4*B9</f>
@@ -3560,7 +3559,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B17">
         <f>-B6*B10</f>
@@ -3569,7 +3568,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18">
         <f>B11*B12</f>
@@ -3578,7 +3577,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B19" s="32">
         <f>SUM(B16:B18)/B5</f>
@@ -3587,7 +3586,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B21" s="22">
         <f>B19/B13</f>

</xml_diff>

<commit_message>
Add parameter sweep analysis for actuator lifting force.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -9,14 +9,83 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
     <sheet name="joints and bearings" sheetId="2" r:id="rId2"/>
     <sheet name="tip vs. slip" sheetId="3" r:id="rId3"/>
+    <sheet name="actuator" sheetId="4" r:id="rId4"/>
+    <sheet name="actuator_diag-ls-friction" sheetId="6" r:id="rId5"/>
+    <sheet name="actuator-diag-slider-friction" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'actuator_diag-ls-friction'!$B$5</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'actuator-diag-slider-friction'!$B$6</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'actuator_diag-ls-friction'!$B$5</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">actuator!$F$5</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'actuator_diag-ls-friction'!$B$18</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'actuator-diag-slider-friction'!$B$18</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="235">
   <si>
     <t>Desktop - simply supported</t>
   </si>
@@ -250,9 +319,6 @@
     <t>conservatively assume load at extreme corner, therefore felt entirely by one foot</t>
   </si>
   <si>
-    <t>desktop to bracket</t>
-  </si>
-  <si>
     <t>bracket to slider</t>
   </si>
   <si>
@@ -617,6 +683,123 @@
   </si>
   <si>
     <t>Material: steel</t>
+  </si>
+  <si>
+    <t>number of motors</t>
+  </si>
+  <si>
+    <t>motor drive voltage, per motor (V)</t>
+  </si>
+  <si>
+    <t>motor drive current, per motor (A)</t>
+  </si>
+  <si>
+    <t>motor efficiency</t>
+  </si>
+  <si>
+    <t>drivetrain efficiency</t>
+  </si>
+  <si>
+    <t>net efficiency, motor to slider</t>
+  </si>
+  <si>
+    <t>power available to lift per motor (W)</t>
+  </si>
+  <si>
+    <t>electrical power input, per motor (W)</t>
+  </si>
+  <si>
+    <t>lifting force at verge of stalling, per motor (N)</t>
+  </si>
+  <si>
+    <t>leadscrew diameter (mm)</t>
+  </si>
+  <si>
+    <t>leadnut coefficient of friction</t>
+  </si>
+  <si>
+    <t>motor torque rating (Nmm)</t>
+  </si>
+  <si>
+    <t>coefficient of friction, slider pads on wood</t>
+  </si>
+  <si>
+    <t>slider effective length (mm)</t>
+  </si>
+  <si>
+    <t>edge loading offset from center of friction (mm)</t>
+  </si>
+  <si>
+    <t>moment resisted by sliders, per slider (Nmm)</t>
+  </si>
+  <si>
+    <t>contact force at each pad (N)</t>
+  </si>
+  <si>
+    <t>frictional force at each pad (N)</t>
+  </si>
+  <si>
+    <t>total frictional force in system, 4 pads in contact (N)</t>
+  </si>
+  <si>
+    <t>igus polymer nut, light oil lubrication</t>
+  </si>
+  <si>
+    <t>total load (N)</t>
+  </si>
+  <si>
+    <t>total actuation force required (N)</t>
+  </si>
+  <si>
+    <t>approximate for sliding contact nut</t>
+  </si>
+  <si>
+    <t>max lifting speed allowed (mm/s)</t>
+  </si>
+  <si>
+    <t>motor datasheet</t>
+  </si>
+  <si>
+    <t>Lifting load capacity</t>
+  </si>
+  <si>
+    <t>ok to lift?</t>
+  </si>
+  <si>
+    <t>Actuation speed (power analysis)</t>
+  </si>
+  <si>
+    <t>wall wart power supply</t>
+  </si>
+  <si>
+    <t>wall wart power supply, total 1A, split between 2 motors, switch-mode so almost 100% efficient</t>
+  </si>
+  <si>
+    <t>approximate for stepper motors</t>
+  </si>
+  <si>
+    <t>max lifting speed allowed (mm/min)</t>
+  </si>
+  <si>
+    <t>Base Analysis</t>
+  </si>
+  <si>
+    <t>Close the loop: what gives? - leadscrew coefficient of friction</t>
+  </si>
+  <si>
+    <t>Close the loop: what gives? - slider coefficient of friction</t>
+  </si>
+  <si>
+    <t>surplus lifting force (N)</t>
+  </si>
+  <si>
+    <t>actual liftable live load = 12 kg</t>
+  </si>
+  <si>
+    <t>Max value allowable before failure to lift, ceteris paribus</t>
+  </si>
+  <si>
+    <t>actual live load lifted = 12kg</t>
   </si>
 </sst>
 </file>
@@ -627,7 +810,7 @@
     <numFmt numFmtId="164" formatCode="0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -719,16 +902,35 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -736,12 +938,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -803,6 +1085,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1154,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,10 +1676,10 @@
         <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1384,7 +1705,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19">
         <v>370</v>
@@ -1395,7 +1716,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1421,7 +1742,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22">
         <v>18</v>
@@ -1466,7 +1787,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B25" s="11">
         <f>((B22+2*B20)*B21^3-B22*B21^3)/12</f>
@@ -1605,7 +1926,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40" s="11">
         <f>B24+B25</f>
@@ -2079,7 +2400,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B95" s="9">
         <f>structure!E87/structure!B94</f>
@@ -2129,10 +2450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F135"/>
+  <dimension ref="A2:F122"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,1267 +2465,1262 @@
     <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>27</v>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <f>(7.8/1000)/10^3</f>
+        <v>7.7999999999999999E-6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <v>2.67</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>250</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <f>0.58*'joints and bearings'!E5</f>
+        <v>145</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <f>B4*B5</f>
+        <v>13.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8">
+        <f>B7*B6</f>
+        <v>53.4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="12">
+        <f>E12/B8</f>
+        <v>2.2661788389513107</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="16">
+        <f>E5/B9</f>
+        <v>110.31786004836633</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <f>structure!E8</f>
+        <v>45.027900000000002</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <f>'joints and bearings'!E9+'joints and bearings'!E10</f>
+        <v>242.02789999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <f>'joints and bearings'!E11/2</f>
+        <v>121.01394999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16">
+        <v>125</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16">
+        <v>11.8</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="E17">
-        <f>(7.8/1000)/10^3</f>
-        <v>7.7999999999999999E-6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
+        <v>130</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B18">
-        <v>2.67</v>
+        <v>12.5</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E18">
-        <v>250</v>
-      </c>
-      <c r="F18" t="s">
-        <v>29</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19">
-        <f>0.58*'joints and bearings'!E18</f>
-        <v>145</v>
-      </c>
-      <c r="F19" t="s">
-        <v>34</v>
+        <v>90</v>
+      </c>
+      <c r="B19" s="11">
+        <f>B16/3</f>
+        <v>41.666666666666664</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20">
-        <f>B17*B18</f>
-        <v>13.35</v>
+        <v>91</v>
+      </c>
+      <c r="B20" s="11">
+        <f>B19*B18</f>
+        <v>520.83333333333326</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="B21">
-        <f>B20*B19</f>
-        <v>53.4</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>12</v>
+        <f>B16/3</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21">
+        <f>50</f>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="12">
-        <f>E25/B21</f>
-        <v>2.2661788389513107</v>
+        <v>95</v>
+      </c>
+      <c r="B22">
+        <f>B19*3</f>
+        <v>125</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="E22">
-        <v>197</v>
+        <f>structure!B19</f>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="16">
-        <f>E18/B22</f>
-        <v>110.31786004836633</v>
+      <c r="A23" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23">
+        <f>B22*B17^3/12</f>
+        <v>60750</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E23">
-        <f>structure!E8</f>
-        <v>45.027900000000002</v>
-      </c>
-      <c r="F23" t="s">
-        <v>17</v>
+        <f>E12</f>
+        <v>121.01394999999999</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <f>B17/2</f>
+        <v>9</v>
+      </c>
       <c r="D24" s="14" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="E24">
-        <f>'joints and bearings'!E22+'joints and bearings'!E23</f>
-        <v>242.02789999999999</v>
+        <f>E23*(E22+E21/2)</f>
+        <v>6050.6974999999993</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25">
+        <f>E25*B18</f>
+        <v>1815.2092499999999</v>
+      </c>
       <c r="D25" s="14" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="E25">
-        <f>'joints and bearings'!E24/2</f>
-        <v>121.01394999999999</v>
+        <f>E24/B21</f>
+        <v>145.21673999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <f>B25*B24/B23</f>
+        <v>0.26891988888888885</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>84</v>
+      <c r="A27" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="9">
+        <f>E17/B26</f>
+        <v>483.41534178497608</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28">
+        <f>E25/B20</f>
+        <v>0.2788161408</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="9">
+        <f>E18/B28</f>
+        <v>38.735203668667957</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" t="s">
         <v>85</v>
       </c>
-      <c r="B28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29">
-        <v>125</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29">
-        <v>11.8</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30">
-        <v>18</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30">
-        <v>130</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31">
-        <v>12.5</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31">
-        <v>10.8</v>
+      <c r="D31" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="11">
-        <f>B29/3</f>
-        <v>41.666666666666664</v>
+        <v>86</v>
+      </c>
+      <c r="B32">
+        <v>125</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32">
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="11">
-        <f>B32*B31</f>
-        <v>520.83333333333326</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="B33">
+        <v>50</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33">
+        <f>E11</f>
+        <v>242.02789999999999</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B34">
-        <f>B29/3</f>
-        <v>41.666666666666664</v>
+        <v>18</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E34">
-        <f>50</f>
-        <v>50</v>
+        <f>E33*E32</f>
+        <v>60506.974999999999</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35">
-        <f>B32*3</f>
-        <v>125</v>
+        <v>90</v>
+      </c>
+      <c r="B35" s="11">
+        <f>B32/3</f>
+        <v>41.666666666666664</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E35">
-        <f>structure!B19</f>
-        <v>25</v>
+        <f>E34/B37</f>
+        <v>1452.1674</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36">
-        <f>B35*B30^3/12</f>
-        <v>60750</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36">
-        <f>E25</f>
-        <v>121.01394999999999</v>
+        <v>91</v>
+      </c>
+      <c r="B36" s="11">
+        <f>B35*B33</f>
+        <v>2083.333333333333</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="B37">
-        <f>B30/2</f>
-        <v>9</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37">
-        <f>E36*(E35+E34/2)</f>
-        <v>6050.6974999999993</v>
+        <f>B32/3</f>
+        <v>41.666666666666664</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="B38">
-        <f>E38*B31</f>
-        <v>1815.2092499999999</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38">
-        <f>E37/B34</f>
-        <v>145.21673999999999</v>
+        <f>B35*3</f>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="B39">
-        <f>B38*B37/B36</f>
-        <v>0.26891988888888885</v>
+        <f>B38*B34^3/12</f>
+        <v>60750</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="9">
-        <f>E30/B39</f>
-        <v>483.41534178497608</v>
+      <c r="A40" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <f>B34/2</f>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B41">
-        <f>E38/B33</f>
-        <v>0.2788161408</v>
+        <f>E35*B33</f>
+        <v>72608.37</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="9">
-        <f>E31/B41</f>
-        <v>38.735203668667957</v>
+      <c r="A42" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42">
+        <f>B41*B40/B39</f>
+        <v>10.756795555555556</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="9">
+        <f>E17/B42</f>
+        <v>12.085383544624401</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>104</v>
+      <c r="A44" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44">
+        <f>E35/B36</f>
+        <v>0.69704035200000014</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45">
-        <v>125</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E45">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46">
-        <v>50</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E46">
-        <f>E24</f>
-        <v>242.02789999999999</v>
-      </c>
-      <c r="F46" t="s">
-        <v>56</v>
+      <c r="A45" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="9">
+        <f>E18/B44</f>
+        <v>15.494081467467179</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47">
-        <v>18</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E47">
-        <f>E46*E45</f>
-        <v>60506.974999999999</v>
+      <c r="A47" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" s="11">
-        <f>B45/3</f>
-        <v>41.666666666666664</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E48">
-        <f>E47/B50</f>
-        <v>1452.1674</v>
+      <c r="A48" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="11">
-        <f>B48*B46</f>
-        <v>2083.333333333333</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B50">
-        <f>B45/3</f>
-        <v>41.666666666666664</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51">
-        <f>B48*3</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B52">
-        <f>B51*B47^3/12</f>
-        <v>60750</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B53">
-        <f>B47/2</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54">
-        <f>E48*B46</f>
-        <v>72608.37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55">
-        <f>B54*B53/B52</f>
-        <v>10.756795555555556</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B56" s="9">
-        <f>E30/B55</f>
-        <v>12.085383544624401</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B57">
-        <f>E48/B49</f>
-        <v>0.69704035200000014</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B58" s="9">
-        <f>E31/B57</f>
-        <v>15.494081467467179</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A49" s="19" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B62">
+      <c r="B49">
         <f>111-10</f>
         <v>101</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="D49" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E50">
+        <f>0.58*E49</f>
+        <v>562.59999999999991</v>
+      </c>
+      <c r="F50" t="s">
         <v>117</v>
       </c>
-      <c r="E62">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53">
+        <f>PI()*B50^2/4</f>
+        <v>19.634954084936208</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E53">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54">
+        <f>E56/B52</f>
+        <v>299.53948019801982</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54">
+        <f>E33</f>
+        <v>242.02789999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55">
+        <f>B54/B53</f>
+        <v>15.255420455901362</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E55">
+        <f>E54*E53</f>
+        <v>60506.974999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="22">
+        <f>E50/B55</f>
+        <v>36.87869512520485</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56">
+        <f>E55/B49</f>
+        <v>599.07896039603963</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59">
+        <f>B51</f>
+        <v>12</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59">
+        <v>11.8</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60">
+        <v>130</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61">
+        <f>B60*B50</f>
+        <v>30</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62">
+        <f>B54/B61</f>
+        <v>9.9846493399339931</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="22">
+        <f>E61/B62</f>
+        <v>1.0816604201416449</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66">
+        <v>3000</v>
+      </c>
+      <c r="C66" t="s">
+        <v>194</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E66">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67">
+        <f>B66/(E66*B50)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68">
+        <v>0.3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69">
+        <f>B67*B68*B52</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B70" s="22">
+        <f>B69/E56</f>
+        <v>2.0030748521141568</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B73" s="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B74" s="30">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75" s="30">
+        <f>PI()*(B73^2-B74^2)/4</f>
+        <v>78.885391531639698</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76" s="30">
+        <f>B67/B75</f>
+        <v>25.353236653428173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="31">
+        <f>E61/B76</f>
+        <v>0.42598111427085439</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="30">
+        <f>B78*PI()*B73</f>
+        <v>678.58401317539528</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B80" s="30">
+        <f>B67/B79</f>
+        <v>2.9473137609610252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" s="31">
+        <f>E59/B80</f>
+        <v>4.0036456777348324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B85">
+        <v>11.7</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E85">
         <v>970</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B86">
         <v>5</v>
       </c>
-      <c r="D63" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="E63">
-        <f>0.58*E62</f>
+      <c r="D86" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E86">
+        <f>0.58*E85</f>
         <v>562.59999999999991</v>
       </c>
-      <c r="F63" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B64">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87">
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B65">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88">
         <v>2</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B66">
-        <f>PI()*B63^2/4</f>
+      <c r="D88" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B89">
+        <f>PI()*B86^2/4</f>
         <v>19.634954084936208</v>
       </c>
-      <c r="D66" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E66">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B67">
-        <f>E69/B65</f>
-        <v>299.53948019801982</v>
-      </c>
-      <c r="D67" s="14" t="s">
+      <c r="D89" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E67">
-        <f>E46</f>
+      <c r="E89">
+        <f>E33</f>
         <v>242.02789999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B68">
-        <f>B67/B66</f>
-        <v>15.255420455901362</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68">
-        <f>E67*E66</f>
-        <v>60506.974999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B69" s="22">
-        <f>E63/B68</f>
-        <v>36.87869512520485</v>
-      </c>
-      <c r="D69" s="26" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B90">
+        <f>E91/B85/B88</f>
+        <v>217.20452564102567</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E90">
+        <f>12+9</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B91">
+        <f>B90/B89</f>
+        <v>11.06213565366386</v>
+      </c>
+      <c r="D91" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E91">
+        <f>E90*E89</f>
+        <v>5082.5859</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B92" s="22">
+        <f>E85/B91</f>
+        <v>87.686503797187555</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E69">
-        <f>E68/B62</f>
-        <v>599.07896039603963</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="D71" s="1" t="s">
+      <c r="B93" s="28">
+        <f>E89/B88</f>
+        <v>121.01394999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B94" s="28">
+        <f>B93/B89</f>
+        <v>6.1631898641841492</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B95" s="22">
+        <f>E86/B94</f>
+        <v>91.283898824764492</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B96" s="28">
+        <f>B90/B120</f>
+        <v>0.29546302493760312</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B97" s="22">
+        <f>E100/B96</f>
+        <v>39.93731534594545</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B72">
-        <f>B64</f>
-        <v>12</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E72">
-        <v>11.8</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="B73">
-        <v>6</v>
-      </c>
-      <c r="C73" t="s">
-        <v>122</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E73">
-        <v>130</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B74">
-        <f>B73*B63</f>
-        <v>30</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="B75">
-        <f>B67/B74</f>
-        <v>9.9846493399339931</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B76" s="22">
-        <f>E74/B75</f>
-        <v>1.0816604201416449</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="D78" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="B79">
-        <v>3000</v>
-      </c>
-      <c r="C79" t="s">
-        <v>195</v>
-      </c>
-      <c r="D79" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="E79">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B80">
-        <f>B79/(E79*B63)</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="B81">
-        <v>0.3</v>
-      </c>
-      <c r="C81" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B82">
-        <f>B80*B81*B65</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="B83" s="22">
-        <f>B82/E69</f>
-        <v>2.0030748521141568</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="B86" s="30">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="B87" s="30">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="B88" s="30">
-        <f>PI()*(B86^2-B87^2)/4</f>
-        <v>78.885391531639698</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B89" s="30">
-        <f>B80/B88</f>
-        <v>25.353236653428173</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B90" s="31">
-        <f>E74/B89</f>
-        <v>0.42598111427085439</v>
-      </c>
-      <c r="C90" s="22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="B91" s="30">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="B92" s="30">
-        <f>B91*PI()*B86</f>
-        <v>678.58401317539528</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B93" s="30">
-        <f>B80/B92</f>
-        <v>2.9473137609610252</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="B94" s="31">
-        <f>E72/B93</f>
-        <v>4.0036456777348324</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D97" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B98">
-        <v>11.7</v>
-      </c>
-      <c r="D98" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="E98">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="B99">
-        <v>5</v>
-      </c>
-      <c r="D99" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="E99">
-        <f>0.58*E98</f>
-        <v>562.59999999999991</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B100">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E100">
+        <v>11.8</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="B101">
-        <v>2</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>143</v>
+        <v>6</v>
+      </c>
+      <c r="C101" t="s">
+        <v>121</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E101">
+        <v>130</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="B102">
-        <f>PI()*B99^2/4</f>
-        <v>19.634954084936208</v>
+        <f>B101*B86</f>
+        <v>30</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="E102">
-        <f>E46</f>
-        <v>242.02789999999999</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="B103">
-        <f>E104/B98/B101</f>
-        <v>217.20452564102567</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E103">
-        <f>12+9</f>
-        <v>21</v>
+        <f>B93/B102</f>
+        <v>4.0337983333333334</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B104">
-        <f>B103/B102</f>
-        <v>11.06213565366386</v>
-      </c>
-      <c r="D104" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="E104">
-        <f>E103*E102</f>
-        <v>5082.5859</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="B105" s="22">
-        <f>E98/B104</f>
-        <v>87.686503797187555</v>
+      <c r="A104" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B104" s="22">
+        <f>E102/B103</f>
+        <v>2.6773772775783291</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B106" s="28">
-        <f>E102/B101</f>
-        <v>121.01394999999999</v>
+      <c r="A106" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D106" s="18" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="B107" s="28">
-        <f>B106/B102</f>
-        <v>6.1631898641841492</v>
+      <c r="A107" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B107">
+        <v>2000</v>
+      </c>
+      <c r="C107" t="s">
+        <v>130</v>
+      </c>
+      <c r="D107" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E107">
+        <v>0.3</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="B108" s="22">
-        <f>E99/B107</f>
-        <v>91.283898824764492</v>
+      <c r="A108" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B108">
+        <f>B107/(E107*B86)</f>
+        <v>1333.3333333333333</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="27" t="s">
+      <c r="A109" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B109">
+        <v>0.3</v>
+      </c>
+      <c r="C109" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B110">
+        <f>B108*B109*B88</f>
+        <v>799.99999999999989</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B111" s="22">
+        <f>B110/B90</f>
+        <v>3.6831645088379115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B114" s="30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B115" s="30">
+        <v>7.93</v>
+      </c>
+      <c r="C115" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B116" s="30">
+        <f>PI()*(B114^2-B115^2)/4</f>
+        <v>83.342604648736568</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B117" s="30">
+        <f>B108/B116</f>
+        <v>15.998220105466141</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B118" s="31">
+        <f>E102/B117</f>
+        <v>0.67507509765476637</v>
+      </c>
+      <c r="C118" s="22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B119" s="30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B120" s="30">
+        <f>B119*PI()*B114</f>
+        <v>735.1326809400116</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="B109" s="28">
-        <f>B103/B133</f>
-        <v>0.29546302493760312</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="B110" s="22">
-        <f>E113/B109</f>
-        <v>39.93731534594545</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B113">
-        <v>18</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E113">
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="B114">
-        <v>6</v>
-      </c>
-      <c r="C114" t="s">
-        <v>122</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E114">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B115">
-        <f>B114*B99</f>
-        <v>30</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E115">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="B116">
-        <f>B106/B115</f>
-        <v>4.0337983333333334</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B117" s="22">
-        <f>E115/B116</f>
-        <v>2.6773772775783291</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="D119" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="B120">
-        <v>2000</v>
-      </c>
-      <c r="C120" t="s">
-        <v>131</v>
-      </c>
-      <c r="D120" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="E120">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B121">
-        <f>B120/(E120*B99)</f>
-        <v>1333.3333333333333</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="B122">
-        <v>0.3</v>
-      </c>
-      <c r="C122" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B123">
-        <f>B121*B122*B101</f>
-        <v>799.99999999999989</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="B124" s="22">
-        <f>B123/B103</f>
-        <v>3.6831645088379115</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="29" t="s">
+      <c r="B121" s="30">
+        <f>B108/B120</f>
+        <v>1.8137315452067844</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="21" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="B127" s="30">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="B128" s="30">
-        <v>7.93</v>
-      </c>
-      <c r="C128" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B129" s="30">
-        <f>PI()*(B127^2-B128^2)/4</f>
-        <v>83.342604648736568</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B130" s="30">
-        <f>B121/B129</f>
-        <v>15.998220105466141</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B131" s="31">
-        <f>E115/B130</f>
-        <v>0.67507509765476637</v>
-      </c>
-      <c r="C131" s="22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="B132" s="30">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="B133" s="30">
-        <f>B132*PI()*B127</f>
-        <v>735.1326809400116</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B134" s="30">
-        <f>B121/B133</f>
-        <v>1.8137315452067844</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="B135" s="31">
-        <f>E113/B134</f>
+      <c r="B122" s="31">
+        <f>E100/B121</f>
         <v>6.5059242263191033</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F29" r:id="rId1"/>
-    <hyperlink ref="F30" r:id="rId2"/>
-    <hyperlink ref="F72" r:id="rId3"/>
-    <hyperlink ref="F73" r:id="rId4"/>
+    <hyperlink ref="F16" r:id="rId1"/>
+    <hyperlink ref="F17" r:id="rId2"/>
+    <hyperlink ref="F59" r:id="rId3"/>
+    <hyperlink ref="F60" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId5"/>
@@ -3415,8 +3731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3427,7 +3743,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1">
         <v>0.25</v>
@@ -3435,18 +3751,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2">
         <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3">
         <v>8.7799999999999994</v>
@@ -3454,7 +3770,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B4" s="13">
         <f>B3*9.81</f>
@@ -3463,19 +3779,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B5" s="13">
         <f>ROUNDUP(398.17,1)</f>
         <v>398.20000000000005</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B6">
         <f>structure!E7</f>
@@ -3484,7 +3800,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <v>500</v>
@@ -3492,7 +3808,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B8">
         <v>500</v>
@@ -3500,7 +3816,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B9">
         <v>250</v>
@@ -3508,18 +3824,18 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B10">
         <v>375</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="13">
         <f>B6+B4</f>
@@ -3528,7 +3844,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12" s="28">
         <v>500</v>
@@ -3536,7 +3852,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="32">
         <f>B1*(B6+B4)</f>
@@ -3545,12 +3861,12 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16">
         <f>-B4*B9</f>
@@ -3559,7 +3875,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17">
         <f>-B6*B10</f>
@@ -3568,7 +3884,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B18">
         <f>B11*B12</f>
@@ -3577,7 +3893,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="32">
         <f>SUM(B16:B18)/B5</f>
@@ -3586,11 +3902,785 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B21" s="22">
         <f>B19/B13</f>
         <v>1.6376330634228966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="55"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="43"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="37">
+        <v>600</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" s="56"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="43"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="37">
+        <v>2</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="43"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="37">
+        <v>10</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="43"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="39">
+        <v>0.25</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="E6" s="56"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="43"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="43"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="40">
+        <f>structure!$E$24</f>
+        <v>45.027900000000002</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="43"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="40">
+        <f>structure!$E$23</f>
+        <v>197</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="43"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="40">
+        <f>B9+B8</f>
+        <v>242.02789999999999</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="43"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="37">
+        <v>100</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="43"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" s="40">
+        <f>250</f>
+        <v>250</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="43"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" s="40">
+        <f>B12*B9/2</f>
+        <v>24625</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="43"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="40">
+        <f>B13/B11</f>
+        <v>246.25</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="43"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15" s="40">
+        <f>B14*B7</f>
+        <v>49.25</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="43"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" s="40">
+        <f>B15*4</f>
+        <v>197</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="43"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="40">
+        <f>B16+B10</f>
+        <v>439.02789999999999</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="43"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="41">
+        <f>B3/(B6*B5)</f>
+        <v>240</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" s="42" t="str">
+        <f>IF(2*B18&gt;B17,"YES","NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="38"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="38"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" s="37">
+        <v>12</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="40">
+        <f>B23*B22</f>
+        <v>6</v>
+      </c>
+      <c r="C24" s="38"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="41">
+        <f>B26*B25</f>
+        <v>0.27</v>
+      </c>
+      <c r="C27" s="38"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" s="41">
+        <f>B24*B27</f>
+        <v>1.62</v>
+      </c>
+      <c r="C28" s="38"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="B29" s="40">
+        <f>((B28*B4)/B17)*1000</f>
+        <v>7.3799410014716615</v>
+      </c>
+      <c r="C29" s="38"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="B30" s="45">
+        <f>B29*60</f>
+        <v>442.79646008829968</v>
+      </c>
+      <c r="C30" s="46"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="50">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="58">
+        <v>0.4278564505307334</v>
+      </c>
+      <c r="C5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="52">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="53">
+        <f>structure!$E$24</f>
+        <v>45.027900000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="53">
+        <f>12*9.81</f>
+        <v>117.72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="53">
+        <f>B8+B7</f>
+        <v>162.74790000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="53">
+        <f>250</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="53">
+        <f>B11*B8/2</f>
+        <v>14715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="53">
+        <f>B12/B10</f>
+        <v>147.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="53">
+        <f>B13*B6</f>
+        <v>29.430000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="53">
+        <f>B14*4</f>
+        <v>117.72000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="53">
+        <f>B15+B9</f>
+        <v>280.46790000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="54">
+        <f>B2/(B5*B4)</f>
+        <v>140.23394978753541</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" s="57">
+        <f>(B17*2)-B16</f>
+        <v>-4.249292260283255E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="50">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="52">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="59">
+        <v>0.53899439517499137</v>
+      </c>
+      <c r="C6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="53">
+        <f>structure!$E$24</f>
+        <v>45.027900000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="53">
+        <f>12*9.81</f>
+        <v>117.72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="53">
+        <f>B8+B7</f>
+        <v>162.74790000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="53">
+        <f>250</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="53">
+        <f>B11*B8/2</f>
+        <v>14715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="53">
+        <f>B12/B10</f>
+        <v>147.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="53">
+        <f>B13*B6</f>
+        <v>79.313025249999981</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="53">
+        <f>B14*4</f>
+        <v>317.25210099999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="53">
+        <f>B15+B9</f>
+        <v>480.00000099999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="54">
+        <f>B2/(B5*B4)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" s="57">
+        <f>(B17*2)-B16</f>
+        <v>-9.9999994063182385E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename worksheets for greater clarity.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -9,80 +9,117 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
     <sheet name="joints and bearings" sheetId="2" r:id="rId2"/>
     <sheet name="tip vs. slip" sheetId="3" r:id="rId3"/>
     <sheet name="actuator" sheetId="4" r:id="rId4"/>
-    <sheet name="actuator_diag-ls-friction" sheetId="6" r:id="rId5"/>
-    <sheet name="actuator-diag-slider-friction" sheetId="5" r:id="rId6"/>
+    <sheet name="ls-friction-sweep" sheetId="6" r:id="rId5"/>
+    <sheet name="slider-friction-sweep" sheetId="5" r:id="rId6"/>
+    <sheet name="min-deviation-sweep" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="4" hidden="1">'actuator_diag-ls-friction'!$B$5</definedName>
-    <definedName name="solver_adj" localSheetId="5" hidden="1">'actuator-diag-slider-friction'!$B$6</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'ls-friction-sweep'!$B$5</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'min-deviation-sweep'!$B$5:$B$6</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'slider-friction-sweep'!$B$6</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'actuator_diag-ls-friction'!$B$5</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'ls-friction-sweep'!$B$5</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'min-deviation-sweep'!$B$18</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">'min-deviation-sweep'!$B$5</definedName>
+    <definedName name="solver_lhs3" localSheetId="6" hidden="1">'min-deviation-sweep'!$B$6</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">actuator!$F$5</definedName>
-    <definedName name="solver_opt" localSheetId="4" hidden="1">'actuator_diag-ls-friction'!$B$18</definedName>
-    <definedName name="solver_opt" localSheetId="5" hidden="1">'actuator-diag-slider-friction'!$B$18</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'ls-friction-sweep'!$B$18</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'min-deviation-sweep'!$B$21</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'slider-friction-sweep'!$B$18</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="6" hidden="1">'min-deviation-sweep'!$B$19</definedName>
+    <definedName name="solver_rhs3" localSheetId="6" hidden="1">'min-deviation-sweep'!$B$20</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -95,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="239">
   <si>
     <t>Desktop - simply supported</t>
   </si>
@@ -800,6 +837,18 @@
   </si>
   <si>
     <t>actual live load lifted = 12kg</t>
+  </si>
+  <si>
+    <t>Close the loop: what gives? - ls or slider coefficient of friction, minimum deviation condition</t>
+  </si>
+  <si>
+    <t>sum of parameter shift from ls and slider frictional coefficients</t>
+  </si>
+  <si>
+    <t>initial estimate for leadscrew frictional coefficient</t>
+  </si>
+  <si>
+    <t>initial estimate for slider frictional coefficient</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1124,6 +1173,12 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3919,7 +3974,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4340,8 +4395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4516,8 +4571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4686,4 +4741,201 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="50">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="59">
+        <v>0.38084951838628106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="59">
+        <v>0.25881286743951232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="53">
+        <f>structure!$E$24</f>
+        <v>45.027900000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="53">
+        <f>12*9.81</f>
+        <v>117.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="53">
+        <f>B8+B7</f>
+        <v>162.74790000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="53">
+        <f>250</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="53">
+        <f>B11*B8/2</f>
+        <v>14715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="53">
+        <f>B12/B10</f>
+        <v>147.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="53">
+        <f>B13*B6</f>
+        <v>38.084313443724241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="53">
+        <f>B14*4</f>
+        <v>152.33725377489696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="53">
+        <f>B15+B9</f>
+        <v>315.08515377489698</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="54">
+        <f>B2/(B5*B4)</f>
+        <v>157.54253872823412</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" s="60">
+        <f>(B17*2)-B16</f>
+        <v>-7.6318428739341471E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19" s="52">
+        <f>B5</f>
+        <v>0.38084951838628106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
+        <v>238</v>
+      </c>
+      <c r="B20" s="52">
+        <f>B6</f>
+        <v>0.25881286743951232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="57">
+        <f>(B5-B19)+(B6-B20)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix minimum deviation parameter sweep. Now uses sum of squares instead of linear sum to force even spread of error.
</commit_message>
<xml_diff>
--- a/design_spreadsheets/Detailed Engineering.xlsx
+++ b/design_spreadsheets/Detailed Engineering.xlsx
@@ -842,22 +842,23 @@
     <t>Close the loop: what gives? - ls or slider coefficient of friction, minimum deviation condition</t>
   </si>
   <si>
-    <t>sum of parameter shift from ls and slider frictional coefficients</t>
-  </si>
-  <si>
     <t>initial estimate for leadscrew frictional coefficient</t>
   </si>
   <si>
     <t>initial estimate for slider frictional coefficient</t>
+  </si>
+  <si>
+    <t>sum sq of parameter shift from ls and slider frictional coefficients</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -1072,7 +1073,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1167,6 +1168,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4437,7 +4441,7 @@
       <c r="A5" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="59">
         <v>0.4278564505307334</v>
       </c>
       <c r="C5" t="s">
@@ -4557,7 +4561,7 @@
       <c r="A18" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="B18" s="57">
+      <c r="B18" s="58">
         <f>(B17*2)-B16</f>
         <v>-4.249292260283255E-7</v>
       </c>
@@ -4621,7 +4625,7 @@
       <c r="A6" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="60">
         <v>0.53899439517499137</v>
       </c>
       <c r="C6" t="s">
@@ -4733,7 +4737,7 @@
       <c r="A18" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="B18" s="57">
+      <c r="B18" s="58">
         <f>(B17*2)-B16</f>
         <v>-9.9999994063182385E-7</v>
       </c>
@@ -4748,12 +4752,13 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4789,16 +4794,16 @@
       <c r="A5" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="59">
-        <v>0.38084951838628106</v>
+      <c r="B5" s="60">
+        <v>0.36766214023330374</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="59">
-        <v>0.25881286743951232</v>
+      <c r="B6" s="60">
+        <v>0.27801344023384295</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4869,7 +4874,7 @@
       </c>
       <c r="B14" s="53">
         <f>B13*B6</f>
-        <v>38.084313443724241</v>
+        <v>40.909677730409989</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4878,7 +4883,7 @@
       </c>
       <c r="B15" s="53">
         <f>B14*4</f>
-        <v>152.33725377489696</v>
+        <v>163.63871092163996</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -4887,7 +4892,7 @@
       </c>
       <c r="B16" s="53">
         <f>B15+B9</f>
-        <v>315.08515377489698</v>
+        <v>326.38661092164</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -4896,43 +4901,41 @@
       </c>
       <c r="B17" s="54">
         <f>B2/(B5*B4)</f>
-        <v>157.54253872823412</v>
+        <v>163.19330557649039</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
         <v>231</v>
       </c>
-      <c r="B18" s="60">
+      <c r="B18" s="61">
         <f>(B17*2)-B16</f>
-        <v>-7.6318428739341471E-5</v>
+        <v>2.3134077764552785E-7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" s="52">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="52">
-        <f>B5</f>
-        <v>0.38084951838628106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
-        <v>238</v>
-      </c>
       <c r="B20" s="52">
-        <f>B6</f>
-        <v>0.25881286743951232</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="48" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B21" s="57">
-        <f>(B5-B19)+(B6-B20)</f>
-        <v>0</v>
+        <f>(B5-B19)^2+(B6-B20)^2</f>
+        <v>1.9930476101401015E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>